<commit_message>
HW: Battery selection spreadsheet updated with Tenpower cells, quantity changed to 25 devices
</commit_message>
<xml_diff>
--- a/hw/Battery.xlsx
+++ b/hw/Battery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\bat_source\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F65BF4-8A0C-4210-833A-174E6553AB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8350C4-5EC1-4C16-BF9F-903481970AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{4068D473-29DE-484D-A592-A1C1CB715333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{4068D473-29DE-484D-A592-A1C1CB715333}"/>
   </bookViews>
   <sheets>
     <sheet name="26650" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>NKON</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Maximum power</t>
+  </si>
+  <si>
+    <t>Tenpower</t>
+  </si>
+  <si>
+    <t>IFR26700-45HE</t>
+  </si>
+  <si>
+    <t>IFR26700-40HE</t>
   </si>
 </sst>
 </file>
@@ -156,12 +165,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,10 +192,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -516,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9511B763-2DED-49AE-AB75-4A0904116107}">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +669,7 @@
         <v>30</v>
       </c>
       <c r="V2">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="X2" t="s">
         <v>30</v>
@@ -722,15 +738,15 @@
       </c>
       <c r="V3">
         <f>V$2*$U3</f>
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="W3">
         <f>IF(AND(V3&gt;=P$2,ISNUMBER(P3)),V3*P3,IF(AND(V3&gt;=O$2,ISNUMBER(O3)),V3*O3,IF(AND(V3&gt;=N$2,ISNUMBER(N3)),V3*N3,IF(AND(V3&gt;=M$2,ISNUMBER(M3)),V3*M3,IF(AND(V3&gt;=L$2,ISNUMBER(L3)),V3*L3,IF(AND(V3&gt;=K$2,ISNUMBER(K3)),V3*K3,IF(AND(V3&gt;=J$2,ISNUMBER(J3)),V3*J3,V3*I3)))))))</f>
-        <v>367.5</v>
+        <v>893.75</v>
       </c>
       <c r="X3">
         <f>W3/V3*U3</f>
-        <v>36.75</v>
+        <v>35.75</v>
       </c>
       <c r="Y3">
         <f>D3*F3*U3</f>
@@ -786,39 +802,39 @@
         <v>3.14</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R7" si="0">ROUNDUP(R$2/D4/H4,2)</f>
+        <f t="shared" ref="R4:R9" si="0">ROUNDUP(R$2/D4/H4,2)</f>
         <v>0.79</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T7" si="1">ROUNDUP(T$2/$D4/$F4,2)</f>
+        <f t="shared" ref="T4:T9" si="1">ROUNDUP(T$2/$D4/$F4,2)</f>
         <v>4.05</v>
       </c>
       <c r="U4">
-        <f t="shared" ref="U4:U7" si="2">ROUNDUP(MAX(T$2/$D4/$F4,R$2/E4/H4),0)</f>
+        <f t="shared" ref="U4:U9" si="2">ROUNDUP(MAX(T$2/$D4/$F4,R$2/E4/H4),0)</f>
         <v>5</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V7" si="3">V$2*$U4</f>
-        <v>50</v>
+        <f t="shared" ref="V4:V9" si="3">V$2*$U4</f>
+        <v>125</v>
       </c>
       <c r="W4">
         <f>IF(AND(V4&gt;=P$2,ISNUMBER(P4)),V4*P4,IF(AND(V4&gt;=O$2,ISNUMBER(O4)),V4*O4,IF(AND(V4&gt;=N$2,ISNUMBER(N4)),V4*N4,IF(AND(V4&gt;=M$2,ISNUMBER(M4)),V4*M4,IF(AND(V4&gt;=L$2,ISNUMBER(L4)),V4*L4,IF(AND(V4&gt;=K$2,ISNUMBER(K4)),V4*K4,IF(AND(V4&gt;=J$2,ISNUMBER(J4)),V4*J4,V4*I4)))))))</f>
-        <v>187</v>
+        <v>442.5</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X7" si="4">W4/V4*U4</f>
-        <v>18.700000000000003</v>
+        <f t="shared" ref="X4:X9" si="4">W4/V4*U4</f>
+        <v>17.7</v>
       </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y7" si="5">D4*F4*U4</f>
+        <f t="shared" ref="Y4:Y9" si="5">D4*F4*U4</f>
         <v>46.4</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z7" si="6">Y4/R$2*60</f>
+        <f t="shared" ref="Z4:Z9" si="6">Y4/R$2*60</f>
         <v>37.120000000000005</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AA7" si="7">E4*H4*U4</f>
+        <f t="shared" ref="AA4:AA9" si="7">E4*H4*U4</f>
         <v>375</v>
       </c>
     </row>
@@ -876,15 +892,15 @@
       </c>
       <c r="V5">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="W5">
         <f>IF(AND(V5&gt;=P$2,ISNUMBER(P5)),V5*P5,IF(AND(V5&gt;=O$2,ISNUMBER(O5)),V5*O5,IF(AND(V5&gt;=N$2,ISNUMBER(N5)),V5*N5,IF(AND(V5&gt;=M$2,ISNUMBER(M5)),V5*M5,IF(AND(V5&gt;=L$2,ISNUMBER(L5)),V5*L5,IF(AND(V5&gt;=K$2,ISNUMBER(K5)),V5*K5,IF(AND(V5&gt;=J$2,ISNUMBER(J5)),V5*J5,V5*I5)))))))</f>
-        <v>90</v>
+        <v>215</v>
       </c>
       <c r="X5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="Y5">
         <f t="shared" si="5"/>
@@ -953,15 +969,15 @@
       </c>
       <c r="V6">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="W6">
         <f>IF(AND(V6&gt;=P$2,ISNUMBER(P6)),V6*P6,IF(AND(V6&gt;=O$2,ISNUMBER(O6)),V6*O6,IF(AND(V6&gt;=N$2,ISNUMBER(N6)),V6*N6,IF(AND(V6&gt;=M$2,ISNUMBER(M6)),V6*M6,IF(AND(V6&gt;=L$2,ISNUMBER(L6)),V6*L6,IF(AND(V6&gt;=K$2,ISNUMBER(K6)),V6*K6,IF(AND(V6&gt;=J$2,ISNUMBER(J6)),V6*J6,V6*I6)))))))</f>
-        <v>111.6</v>
+        <v>269</v>
       </c>
       <c r="X6">
         <f t="shared" si="4"/>
-        <v>11.16</v>
+        <v>10.76</v>
       </c>
       <c r="Y6">
         <f t="shared" si="5"/>
@@ -1030,11 +1046,11 @@
       </c>
       <c r="V7">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="W7">
         <f>IF(AND(V7&gt;=P$2,ISNUMBER(P7)),V7*P7,IF(AND(V7&gt;=O$2,ISNUMBER(O7)),V7*O7,IF(AND(V7&gt;=N$2,ISNUMBER(N7)),V7*N7,IF(AND(V7&gt;=M$2,ISNUMBER(M7)),V7*M7,IF(AND(V7&gt;=L$2,ISNUMBER(L7)),V7*L7,IF(AND(V7&gt;=K$2,ISNUMBER(K7)),V7*K7,IF(AND(V7&gt;=J$2,ISNUMBER(J7)),V7*J7,V7*I7)))))))</f>
-        <v>89.7</v>
+        <v>224.25000000000003</v>
       </c>
       <c r="X7">
         <f t="shared" si="4"/>
@@ -1051,6 +1067,174 @@
       <c r="AA7">
         <f t="shared" si="7"/>
         <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>3.2</v>
+      </c>
+      <c r="E8">
+        <v>2.5</v>
+      </c>
+      <c r="F8">
+        <v>4.45</v>
+      </c>
+      <c r="G8">
+        <v>4.5</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3">
+        <f>$M8*$M$2/I$2</f>
+        <v>195</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:L9" si="8">$M8*$M$2/J$2</f>
+        <v>19.5</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="8"/>
+        <v>6.5</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="8"/>
+        <v>3.9</v>
+      </c>
+      <c r="M8">
+        <v>1.95</v>
+      </c>
+      <c r="N8">
+        <v>1.85</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>2.61</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>2.6399999999999997</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ref="W8:W9" si="9">IF(AND(V8&gt;=P$2,ISNUMBER(P8)),V8*P8,IF(AND(V8&gt;=O$2,ISNUMBER(O8)),V8*O8,IF(AND(V8&gt;=N$2,ISNUMBER(N8)),V8*N8,IF(AND(V8&gt;=M$2,ISNUMBER(M8)),V8*M8,IF(AND(V8&gt;=L$2,ISNUMBER(L8)),V8*L8,IF(AND(V8&gt;=K$2,ISNUMBER(K8)),V8*K8,IF(AND(V8&gt;=J$2,ISNUMBER(J8)),V8*J8,V8*I8)))))))</f>
+        <v>195</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="4"/>
+        <v>7.8</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="5"/>
+        <v>56.960000000000008</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="6"/>
+        <v>45.568000000000005</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>3.2</v>
+      </c>
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+      <c r="F9">
+        <v>3.95</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3">
+        <f>$M9*$M$2/I$2</f>
+        <v>185</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="8"/>
+        <v>18.5</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="8"/>
+        <v>6.166666666666667</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="8"/>
+        <v>3.7</v>
+      </c>
+      <c r="M9">
+        <v>1.85</v>
+      </c>
+      <c r="N9">
+        <v>1.75</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>2.9299999999999997</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="9"/>
+        <v>185</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="4"/>
+        <v>7.4</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="5"/>
+        <v>50.56</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="6"/>
+        <v>40.448</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="7"/>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1063,6 +1247,8 @@
     <hyperlink ref="C5" r:id="rId3" xr:uid="{4B908EB6-23E7-412D-9B96-2B984F1898FB}"/>
     <hyperlink ref="C6" r:id="rId4" xr:uid="{64C73AAC-4023-488A-AF48-2D2CE40C8C10}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{5D49E683-A6E3-499A-BF53-E9263AD00310}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{FC179B28-0309-44B7-B00A-68923ADB5302}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{CC8A62E8-449B-4B7D-BAA9-FEDD2B404A9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>